<commit_message>
add res boundary attack for SEED 999
</commit_message>
<xml_diff>
--- a/results/SEED_999/result.xlsx
+++ b/results/SEED_999/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -800,130 +852,154 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.676121234893799</v>
+        <v>4.676124095916748</v>
       </c>
       <c r="D4" t="n">
-        <v>3.700270891189575</v>
+        <v>3.700276374816895</v>
       </c>
       <c r="E4" t="n">
-        <v>4.520951141010631</v>
+        <v>4.520952744917436</v>
       </c>
       <c r="F4" t="n">
-        <v>4.499168656089089</v>
+        <v>4.499170476740057</v>
       </c>
       <c r="G4" t="n">
-        <v>4.642141558907249</v>
+        <v>4.642143899744207</v>
       </c>
       <c r="H4" t="n">
-        <v>4.966532187028364</v>
+        <v>4.96653379093517</v>
       </c>
       <c r="I4" t="n">
-        <v>5.474898208271373</v>
+        <v>5.474897102876143</v>
       </c>
       <c r="J4" t="n">
-        <v>7.284216989170421</v>
+        <v>7.284216382286766</v>
       </c>
       <c r="K4" t="n">
-        <v>9.582349148663608</v>
+        <v>9.582347219640559</v>
       </c>
       <c r="L4" t="n">
-        <v>18.73878513682972</v>
+        <v>18.73878260092302</v>
       </c>
       <c r="M4" t="n">
-        <v>4.56476506319913</v>
+        <v>4.564767750826749</v>
       </c>
       <c r="N4" t="n">
-        <v>4.533811309120872</v>
+        <v>4.533812262795188</v>
       </c>
       <c r="O4" t="n">
-        <v>4.562311562624845</v>
+        <v>4.562313556671143</v>
       </c>
       <c r="P4" t="n">
-        <v>4.654838431965221</v>
+        <v>4.65484129298817</v>
       </c>
       <c r="Q4" t="n">
-        <v>4.80892411145297</v>
+        <v>4.808925802057439</v>
       </c>
       <c r="R4" t="n">
-        <v>5.57801342010498</v>
+        <v>5.578014893965288</v>
       </c>
       <c r="S4" t="n">
-        <v>6.762895237315785</v>
+        <v>6.762894023548473</v>
       </c>
       <c r="T4" t="n">
-        <v>12.44454704631459</v>
+        <v>12.44454578919844</v>
       </c>
       <c r="U4" t="n">
-        <v>4.56476506319913</v>
+        <v>4.564767750826749</v>
       </c>
       <c r="V4" t="n">
-        <v>4.535321625796231</v>
+        <v>4.535323749889027</v>
       </c>
       <c r="W4" t="n">
-        <v>4.56456318768588</v>
+        <v>4.564564574848522</v>
       </c>
       <c r="X4" t="n">
-        <v>4.656448754397306</v>
+        <v>4.656451311978427</v>
       </c>
       <c r="Y4" t="n">
-        <v>4.816559314727783</v>
+        <v>4.816561178727583</v>
       </c>
       <c r="Z4" t="n">
-        <v>5.398611849004572</v>
+        <v>5.398612282492897</v>
       </c>
       <c r="AA4" t="n">
-        <v>6.758034576069225</v>
+        <v>6.758034359325062</v>
       </c>
       <c r="AB4" t="n">
-        <v>12.22071762518449</v>
+        <v>12.22071801532399</v>
       </c>
       <c r="AC4" t="n">
-        <v>6.040481567382812</v>
+        <v>6.040483474731445</v>
       </c>
       <c r="AD4" t="n">
-        <v>7.446005344390869</v>
+        <v>7.446007251739502</v>
       </c>
       <c r="AE4" t="n">
-        <v>8.859755516052246</v>
+        <v>8.859757423400879</v>
       </c>
       <c r="AF4" t="n">
-        <v>10.27543544769287</v>
+        <v>10.27543640136719</v>
       </c>
       <c r="AG4" t="n">
-        <v>11.69254970550537</v>
+        <v>11.69255065917969</v>
       </c>
       <c r="AH4" t="n">
-        <v>15.239013671875</v>
+        <v>15.23901653289795</v>
       </c>
       <c r="AI4" t="n">
-        <v>18.78341102600098</v>
+        <v>18.78341484069824</v>
       </c>
       <c r="AJ4" t="n">
         <v>32.86657333374023</v>
       </c>
       <c r="AK4" t="n">
-        <v>6.101568222045898</v>
+        <v>6.101570606231689</v>
       </c>
       <c r="AL4" t="n">
-        <v>7.528539657592773</v>
+        <v>7.528542041778564</v>
       </c>
       <c r="AM4" t="n">
-        <v>8.956755638122559</v>
+        <v>8.956756591796875</v>
       </c>
       <c r="AN4" t="n">
-        <v>10.38606643676758</v>
+        <v>10.38606929779053</v>
       </c>
       <c r="AO4" t="n">
-        <v>11.81589984893799</v>
+        <v>11.81590175628662</v>
       </c>
       <c r="AP4" t="n">
-        <v>15.39207363128662</v>
+        <v>15.39207553863525</v>
       </c>
       <c r="AQ4" t="n">
         <v>18.9613208770752</v>
       </c>
       <c r="AR4" t="n">
         <v>33.04644775390625</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>4.711726665496826</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>4.761361122131348</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>4.775956630706787</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>4.868701457977295</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>4.993381977081299</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>5.384127616882324</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>5.428856372833252</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>7.522520065307617</v>
       </c>
     </row>
     <row r="5">
@@ -934,130 +1010,154 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5.814027647033401</v>
+        <v>5.814030927630279</v>
       </c>
       <c r="D5" t="n">
-        <v>4.900428963393772</v>
+        <v>4.900436358582428</v>
       </c>
       <c r="E5" t="n">
-        <v>5.651026852070916</v>
+        <v>5.651029085174697</v>
       </c>
       <c r="F5" t="n">
-        <v>5.697226191334174</v>
+        <v>5.697228086948995</v>
       </c>
       <c r="G5" t="n">
-        <v>5.946140887878054</v>
+        <v>5.94614317597357</v>
       </c>
       <c r="H5" t="n">
-        <v>6.374927834528423</v>
+        <v>6.374929183237306</v>
       </c>
       <c r="I5" t="n">
-        <v>6.95068091419805</v>
+        <v>6.950680947968711</v>
       </c>
       <c r="J5" t="n">
-        <v>8.813669389647389</v>
+        <v>8.813670290839985</v>
       </c>
       <c r="K5" t="n">
-        <v>11.01840959360068</v>
+        <v>11.01840837822166</v>
       </c>
       <c r="L5" t="n">
-        <v>20.31228915855574</v>
+        <v>20.31228702317167</v>
       </c>
       <c r="M5" t="n">
-        <v>5.739486789159455</v>
+        <v>5.739490112612383</v>
       </c>
       <c r="N5" t="n">
-        <v>5.764238260728304</v>
+        <v>5.764239407906405</v>
       </c>
       <c r="O5" t="n">
-        <v>5.886697340835986</v>
+        <v>5.886699657875642</v>
       </c>
       <c r="P5" t="n">
-        <v>6.102656393805359</v>
+        <v>6.102658939288982</v>
       </c>
       <c r="Q5" t="n">
-        <v>6.401570324583307</v>
+        <v>6.401572227522283</v>
       </c>
       <c r="R5" t="n">
-        <v>7.431895105673697</v>
+        <v>7.431896573979799</v>
       </c>
       <c r="S5" t="n">
-        <v>8.741423756816738</v>
+        <v>8.741423565691573</v>
       </c>
       <c r="T5" t="n">
-        <v>14.87752604818041</v>
+        <v>14.87752597151311</v>
       </c>
       <c r="U5" t="n">
-        <v>5.739486789159455</v>
+        <v>5.739490112612383</v>
       </c>
       <c r="V5" t="n">
-        <v>5.765007037385209</v>
+        <v>5.765009532455154</v>
       </c>
       <c r="W5" t="n">
-        <v>5.887341469696882</v>
+        <v>5.88734341772001</v>
       </c>
       <c r="X5" t="n">
-        <v>6.104295329901868</v>
+        <v>6.104297782293159</v>
       </c>
       <c r="Y5" t="n">
-        <v>6.406013987410232</v>
+        <v>6.406016034460116</v>
       </c>
       <c r="Z5" t="n">
-        <v>7.209971639443533</v>
+        <v>7.209972188617448</v>
       </c>
       <c r="AA5" t="n">
-        <v>8.764857231083672</v>
+        <v>8.764858136000154</v>
       </c>
       <c r="AB5" t="n">
-        <v>14.66958530529957</v>
+        <v>14.66958612825128</v>
       </c>
       <c r="AC5" t="n">
-        <v>6.978098803760166</v>
+        <v>6.978101810428749</v>
       </c>
       <c r="AD5" t="n">
-        <v>8.222274894660199</v>
+        <v>8.222277214393348</v>
       </c>
       <c r="AE5" t="n">
-        <v>9.516142131114389</v>
+        <v>9.516144536309728</v>
       </c>
       <c r="AF5" t="n">
-        <v>10.84247575028452</v>
+        <v>10.84247645394247</v>
       </c>
       <c r="AG5" t="n">
-        <v>12.19091060551268</v>
+        <v>12.1909131088183</v>
       </c>
       <c r="AH5" t="n">
-        <v>15.62065857655286</v>
+        <v>15.62066004180366</v>
       </c>
       <c r="AI5" t="n">
-        <v>19.09253525186611</v>
+        <v>19.0925368502697</v>
       </c>
       <c r="AJ5" t="n">
         <v>33.0621529400499</v>
       </c>
       <c r="AK5" t="n">
-        <v>7.003240107926998</v>
+        <v>7.003243103801785</v>
       </c>
       <c r="AL5" t="n">
-        <v>8.270256835934674</v>
+        <v>8.270259603464174</v>
       </c>
       <c r="AM5" t="n">
-        <v>9.584880095892526</v>
+        <v>9.584882483839012</v>
       </c>
       <c r="AN5" t="n">
-        <v>10.93030210979668</v>
+        <v>10.9303055998161</v>
       </c>
       <c r="AO5" t="n">
-        <v>12.29642269558096</v>
+        <v>12.29642455695011</v>
       </c>
       <c r="AP5" t="n">
-        <v>15.76589164092531</v>
+        <v>15.76589454443143</v>
       </c>
       <c r="AQ5" t="n">
-        <v>19.27115489244669</v>
+        <v>19.27115647603506</v>
       </c>
       <c r="AR5" t="n">
-        <v>33.28733439101688</v>
+        <v>33.28733255743185</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>5.849863373554789</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>5.888527737145577</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>5.903361911169605</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>5.98975292021015</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>6.156125759671945</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>6.67196190663539</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>6.552792590091629</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>9.570957806688019</v>
       </c>
     </row>
     <row r="6">
@@ -1068,55 +1168,55 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9996496438980103</v>
+        <v>0.9996495246887207</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9996908903121948</v>
+        <v>0.9996910095214844</v>
       </c>
       <c r="E6" t="n">
         <v>0.9996278285980225</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9995689392089844</v>
+        <v>0.9995688796043396</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9994733929634094</v>
+        <v>0.9994732737541199</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9993417263031006</v>
+        <v>0.9993415474891663</v>
       </c>
       <c r="I6" t="n">
         <v>0.9991739988327026</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9986042976379395</v>
+        <v>0.998604416847229</v>
       </c>
       <c r="K6" t="n">
         <v>0.9978241920471191</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9929627776145935</v>
+        <v>0.9929625391960144</v>
       </c>
       <c r="M6" t="n">
         <v>0.9996389150619507</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9996087551116943</v>
+        <v>0.9996086359024048</v>
       </c>
       <c r="O6" t="n">
         <v>0.9995591640472412</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9994901418685913</v>
+        <v>0.9994899034500122</v>
       </c>
       <c r="Q6" t="n">
         <v>0.9994019269943237</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9991001486778259</v>
+        <v>0.9990999698638916</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9986848831176758</v>
+        <v>0.9986847639083862</v>
       </c>
       <c r="T6" t="n">
         <v>0.9960128664970398</v>
@@ -1128,31 +1228,31 @@
         <v>0.9996091723442078</v>
       </c>
       <c r="W6" t="n">
-        <v>0.9995605945587158</v>
+        <v>0.9995604753494263</v>
       </c>
       <c r="X6" t="n">
         <v>0.9994925856590271</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.9994056820869446</v>
+        <v>0.999405562877655</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.9991755485534668</v>
+        <v>0.9991753697395325</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.9986935257911682</v>
+        <v>0.9986934065818787</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.9961554408073425</v>
+        <v>0.996155321598053</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.9995036721229553</v>
+        <v>0.999503493309021</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.999306321144104</v>
+        <v>0.9993062615394592</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.9990563988685608</v>
+        <v>0.999056339263916</v>
       </c>
       <c r="AF6" t="n">
         <v>0.9987521171569824</v>
@@ -1161,28 +1261,28 @@
         <v>0.9983921647071838</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.9972387552261353</v>
+        <v>0.9972386360168457</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.9957066774368286</v>
+        <v>0.9957065582275391</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.9854373931884766</v>
+        <v>0.9854371547698975</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.9995003938674927</v>
+        <v>0.9995002746582031</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.9992997050285339</v>
+        <v>0.9992996454238892</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.9990458488464355</v>
+        <v>0.999045729637146</v>
       </c>
       <c r="AN6" t="n">
         <v>0.9987375140190125</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.9983734488487244</v>
+        <v>0.9983733296394348</v>
       </c>
       <c r="AP6" t="n">
         <v>0.9972080588340759</v>
@@ -1192,6 +1292,30 @@
       </c>
       <c r="AR6" t="n">
         <v>0.9854254126548767</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0.9996455311775208</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.9996346831321716</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9996383190155029</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9996296167373657</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995920062065125</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9994946718215942</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9995133876800537</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9989163875579834</v>
       </c>
     </row>
     <row r="7">
@@ -1206,130 +1330,154 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.090191841125488</v>
+        <v>3.090195655822754</v>
       </c>
       <c r="D7" t="n">
-        <v>3.652654409408569</v>
+        <v>3.65265679359436</v>
       </c>
       <c r="E7" t="n">
-        <v>2.716965415261008</v>
+        <v>2.716966542330655</v>
       </c>
       <c r="F7" t="n">
-        <v>2.58195651661266</v>
+        <v>2.581958684054288</v>
       </c>
       <c r="G7" t="n">
-        <v>2.718356522646817</v>
+        <v>2.718356652693315</v>
       </c>
       <c r="H7" t="n">
-        <v>3.09484711560336</v>
+        <v>3.094848242673007</v>
       </c>
       <c r="I7" t="n">
-        <v>3.699335531754927</v>
+        <v>3.699334578080611</v>
       </c>
       <c r="J7" t="n">
-        <v>5.673383409326727</v>
+        <v>5.67338262904774</v>
       </c>
       <c r="K7" t="n">
-        <v>7.80037784576416</v>
+        <v>7.800378062508323</v>
       </c>
       <c r="L7" t="n">
-        <v>15.77603595907038</v>
+        <v>15.77603806148876</v>
       </c>
       <c r="M7" t="n">
-        <v>3.055491534146396</v>
+        <v>3.055493831634521</v>
       </c>
       <c r="N7" t="n">
-        <v>3.098951209675182</v>
+        <v>3.09895489432595</v>
       </c>
       <c r="O7" t="n">
-        <v>3.245389461517334</v>
+        <v>3.245391152121804</v>
       </c>
       <c r="P7" t="n">
-        <v>3.497366471724077</v>
+        <v>3.497367165305398</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.855223699049516</v>
+        <v>3.855226430025968</v>
       </c>
       <c r="R7" t="n">
-        <v>5.040690812197599</v>
+        <v>5.040691245685924</v>
       </c>
       <c r="S7" t="n">
-        <v>6.461549065329812</v>
+        <v>6.461548501794988</v>
       </c>
       <c r="T7" t="n">
-        <v>12.53790155324069</v>
+        <v>12.53790057789196</v>
       </c>
       <c r="U7" t="n">
-        <v>2.716965415261008</v>
+        <v>2.716966542330655</v>
       </c>
       <c r="V7" t="n">
-        <v>2.582241231744939</v>
+        <v>2.582242879000577</v>
       </c>
       <c r="W7" t="n">
-        <v>2.714796369726008</v>
+        <v>2.714795199307528</v>
       </c>
       <c r="X7" t="n">
-        <v>3.080373547293923</v>
+        <v>3.080372897061435</v>
       </c>
       <c r="Y7" t="n">
-        <v>3.659885319796476</v>
+        <v>3.659884344447743</v>
       </c>
       <c r="Z7" t="n">
-        <v>5.137606078928167</v>
+        <v>5.141442580656572</v>
       </c>
       <c r="AA7" t="n">
-        <v>7.555836742574519</v>
+        <v>7.559678077697754</v>
       </c>
       <c r="AB7" t="n">
-        <v>15.07243145595897</v>
+        <v>15.07042158733715</v>
       </c>
       <c r="AC7" t="n">
-        <v>4.394396305084229</v>
+        <v>4.39439868927002</v>
       </c>
       <c r="AD7" t="n">
-        <v>5.772855281829834</v>
+        <v>5.772858142852783</v>
       </c>
       <c r="AE7" t="n">
-        <v>7.164175033569336</v>
+        <v>7.164176940917969</v>
       </c>
       <c r="AF7" t="n">
-        <v>8.556443214416504</v>
+        <v>8.556445121765137</v>
       </c>
       <c r="AG7" t="n">
-        <v>9.953130722045898</v>
+        <v>9.953133583068848</v>
       </c>
       <c r="AH7" t="n">
-        <v>13.45127010345459</v>
+        <v>13.45127201080322</v>
       </c>
       <c r="AI7" t="n">
-        <v>16.94616508483887</v>
+        <v>16.9461669921875</v>
       </c>
       <c r="AJ7" t="n">
-        <v>30.83474731445312</v>
+        <v>30.83474922180176</v>
       </c>
       <c r="AK7" t="n">
-        <v>5.058418750762939</v>
+        <v>5.058421611785889</v>
       </c>
       <c r="AL7" t="n">
-        <v>7.027503490447998</v>
+        <v>7.027505874633789</v>
       </c>
       <c r="AM7" t="n">
-        <v>8.997326850891113</v>
+        <v>8.997329711914062</v>
       </c>
       <c r="AN7" t="n">
-        <v>10.96603393554688</v>
+        <v>10.96603679656982</v>
       </c>
       <c r="AO7" t="n">
-        <v>12.92952632904053</v>
+        <v>12.92952919006348</v>
       </c>
       <c r="AP7" t="n">
         <v>17.82774543762207</v>
       </c>
       <c r="AQ7" t="n">
-        <v>22.6911678314209</v>
+        <v>22.69116973876953</v>
       </c>
       <c r="AR7" t="n">
         <v>41.66017150878906</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>3.208371639251709</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>3.397868394851685</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3.772894859313965</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>4.15678596496582</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>4.336008071899414</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>5.759581089019775</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>6.832229614257812</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>11.9419469833374</v>
       </c>
     </row>
     <row r="8">
@@ -1340,130 +1488,154 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.02226901076931</v>
+        <v>4.022272330148218</v>
       </c>
       <c r="D8" t="n">
-        <v>4.72904360886954</v>
+        <v>4.729046230491099</v>
       </c>
       <c r="E8" t="n">
-        <v>3.668942437381893</v>
+        <v>3.668944537113288</v>
       </c>
       <c r="F8" t="n">
-        <v>3.575744977810875</v>
+        <v>3.57574751877034</v>
       </c>
       <c r="G8" t="n">
-        <v>3.762352178802287</v>
+        <v>3.762352234919155</v>
       </c>
       <c r="H8" t="n">
-        <v>4.192281187952942</v>
+        <v>4.192282070187948</v>
       </c>
       <c r="I8" t="n">
-        <v>4.796974953461031</v>
+        <v>4.796974511377022</v>
       </c>
       <c r="J8" t="n">
-        <v>6.720374062777885</v>
+        <v>6.720373859946557</v>
       </c>
       <c r="K8" t="n">
-        <v>8.878394994946307</v>
+        <v>8.878395451494335</v>
       </c>
       <c r="L8" t="n">
-        <v>17.53632318351933</v>
+        <v>17.5363260596243</v>
       </c>
       <c r="M8" t="n">
-        <v>3.985496818521693</v>
+        <v>3.985499669846025</v>
       </c>
       <c r="N8" t="n">
-        <v>4.06250379586853</v>
+        <v>4.062506941490138</v>
       </c>
       <c r="O8" t="n">
-        <v>4.248014431525243</v>
+        <v>4.248016533108602</v>
       </c>
       <c r="P8" t="n">
-        <v>4.529788856187378</v>
+        <v>4.529789932915188</v>
       </c>
       <c r="Q8" t="n">
-        <v>4.888655355757581</v>
+        <v>4.888658602871444</v>
       </c>
       <c r="R8" t="n">
-        <v>6.034488875187811</v>
+        <v>6.034490952911217</v>
       </c>
       <c r="S8" t="n">
-        <v>7.39750759746923</v>
+        <v>7.39750794416439</v>
       </c>
       <c r="T8" t="n">
-        <v>13.61071885413609</v>
+        <v>13.61071801738874</v>
       </c>
       <c r="U8" t="n">
-        <v>3.668942437381893</v>
+        <v>3.668944537113288</v>
       </c>
       <c r="V8" t="n">
-        <v>3.574045616161662</v>
+        <v>3.574047066905208</v>
       </c>
       <c r="W8" t="n">
-        <v>3.759588040449787</v>
+        <v>3.7595875465299</v>
       </c>
       <c r="X8" t="n">
-        <v>4.183803593508613</v>
+        <v>4.183802413918993</v>
       </c>
       <c r="Y8" t="n">
-        <v>4.769169311181016</v>
+        <v>4.769168444137398</v>
       </c>
       <c r="Z8" t="n">
-        <v>6.218853907239165</v>
+        <v>6.220393908284706</v>
       </c>
       <c r="AA8" t="n">
-        <v>8.686833978239664</v>
+        <v>8.687664087523665</v>
       </c>
       <c r="AB8" t="n">
-        <v>16.92500768576405</v>
+        <v>16.92488189482743</v>
       </c>
       <c r="AC8" t="n">
-        <v>5.125773301748525</v>
+        <v>5.125775720459314</v>
       </c>
       <c r="AD8" t="n">
-        <v>6.348822909614544</v>
+        <v>6.348826214294766</v>
       </c>
       <c r="AE8" t="n">
-        <v>7.635300729521045</v>
+        <v>7.635302977780253</v>
       </c>
       <c r="AF8" t="n">
-        <v>8.957865101014233</v>
+        <v>8.957866804409791</v>
       </c>
       <c r="AG8" t="n">
-        <v>10.30050757185261</v>
+        <v>10.30051016423724</v>
       </c>
       <c r="AH8" t="n">
-        <v>13.71428411347516</v>
+        <v>13.71428578240531</v>
       </c>
       <c r="AI8" t="n">
-        <v>17.16583862282877</v>
+        <v>17.16584128954169</v>
       </c>
       <c r="AJ8" t="n">
-        <v>31.03729859070524</v>
+        <v>31.03729760745026</v>
       </c>
       <c r="AK8" t="n">
-        <v>5.659461021506825</v>
+        <v>5.659463380642721</v>
       </c>
       <c r="AL8" t="n">
-        <v>7.460902476603005</v>
+        <v>7.460905033060903</v>
       </c>
       <c r="AM8" t="n">
-        <v>9.332594524388201</v>
+        <v>9.332598203136756</v>
       </c>
       <c r="AN8" t="n">
-        <v>11.23812205255248</v>
+        <v>11.23812544697788</v>
       </c>
       <c r="AO8" t="n">
-        <v>13.15880192088794</v>
+        <v>13.15880424006377</v>
       </c>
       <c r="AP8" t="n">
-        <v>17.9965672928526</v>
+        <v>17.99656898859691</v>
       </c>
       <c r="AQ8" t="n">
-        <v>22.83334209506941</v>
+        <v>22.83334343160513</v>
       </c>
       <c r="AR8" t="n">
-        <v>41.85075382478941</v>
+        <v>41.85075674159011</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>4.121666688550143</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>4.309978024101435</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>4.733208540941442</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>5.295398247486897</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>5.365624879138303</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>7.205592727794008</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>8.594566722554285</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>15.09123812480767</v>
       </c>
     </row>
     <row r="9">
@@ -1474,7 +1646,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9997979998588562</v>
+        <v>0.9997978806495667</v>
       </c>
       <c r="D9" t="n">
         <v>0.9998219609260559</v>
@@ -1483,10 +1655,10 @@
         <v>0.9997962117195129</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9997788071632385</v>
+        <v>0.9997785687446594</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9997455477714539</v>
+        <v>0.9997454881668091</v>
       </c>
       <c r="H9" t="n">
         <v>0.999696671962738</v>
@@ -1498,16 +1670,16 @@
         <v>0.9994072318077087</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9990874528884888</v>
+        <v>0.9990872144699097</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9969233274459839</v>
+        <v>0.9969231486320496</v>
       </c>
       <c r="M9" t="n">
-        <v>0.999798059463501</v>
+        <v>0.9997979402542114</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9997815489768982</v>
+        <v>0.9997813701629639</v>
       </c>
       <c r="O9" t="n">
         <v>0.9997484683990479</v>
@@ -1519,19 +1691,19 @@
         <v>0.9996333122253418</v>
       </c>
       <c r="R9" t="n">
-        <v>0.9993970990180969</v>
+        <v>0.9993970394134521</v>
       </c>
       <c r="S9" t="n">
         <v>0.9990597367286682</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9966990947723389</v>
+        <v>0.9966990351676941</v>
       </c>
       <c r="U9" t="n">
         <v>0.9997962117195129</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9997791647911072</v>
+        <v>0.9997789859771729</v>
       </c>
       <c r="W9" t="n">
         <v>0.9997458457946777</v>
@@ -1540,55 +1712,55 @@
         <v>0.9996967315673828</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.999633252620697</v>
+        <v>0.9996330738067627</v>
       </c>
       <c r="Z9" t="n">
         <v>0.9994613528251648</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.9990856051445007</v>
+        <v>0.9990858435630798</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.9967852234840393</v>
+        <v>0.9967865347862244</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.9996773600578308</v>
+        <v>0.9996771812438965</v>
       </c>
       <c r="AD9" t="n">
         <v>0.9994996786117554</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.9992638230323792</v>
+        <v>0.9992637038230896</v>
       </c>
       <c r="AF9" t="n">
         <v>0.9989684820175171</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.9986143112182617</v>
+        <v>0.9986140727996826</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.9974568486213684</v>
+        <v>0.9974567294120789</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.9958980083465576</v>
+        <v>0.9958978295326233</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.9853779077529907</v>
+        <v>0.9853777289390564</v>
       </c>
       <c r="AK9" t="n">
         <v>0.9996119141578674</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.9993173480033875</v>
+        <v>0.9993172883987427</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.9989106059074402</v>
+        <v>0.9989105463027954</v>
       </c>
       <c r="AN9" t="n">
         <v>0.9983879923820496</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.9977486729621887</v>
+        <v>0.9977486133575439</v>
       </c>
       <c r="AP9" t="n">
         <v>0.9956093430519104</v>
@@ -1597,7 +1769,31 @@
         <v>0.9926638603210449</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.9722660779953003</v>
+        <v>0.9722659587860107</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0.9997861385345459</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997575283050537</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.999695360660553</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996019005775452</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9995802640914917</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9991702437400818</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9987583756446838</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.996002197265625</v>
       </c>
     </row>
     <row r="10">
@@ -1615,94 +1811,94 @@
         <v>3.0233154296875</v>
       </c>
       <c r="D10" t="n">
-        <v>1.65008020401001</v>
+        <v>1.650080561637878</v>
       </c>
       <c r="E10" t="n">
-        <v>2.968636512756348</v>
+        <v>2.968636816198176</v>
       </c>
       <c r="F10" t="n">
-        <v>2.979502807963978</v>
+        <v>2.979503501545299</v>
       </c>
       <c r="G10" t="n">
-        <v>3.056701616807417</v>
+        <v>3.056702136993408</v>
       </c>
       <c r="H10" t="n">
-        <v>3.197386134754528</v>
+        <v>3.19738600470803</v>
       </c>
       <c r="I10" t="n">
-        <v>3.411386706612327</v>
+        <v>3.411386966705322</v>
       </c>
       <c r="J10" t="n">
-        <v>4.250914356925271</v>
+        <v>4.250914031809026</v>
       </c>
       <c r="K10" t="n">
-        <v>5.332047679207542</v>
+        <v>5.332046703858809</v>
       </c>
       <c r="L10" t="n">
-        <v>9.904455531727184</v>
+        <v>9.904454296285456</v>
       </c>
       <c r="M10" t="n">
-        <v>2.794133012945002</v>
+        <v>2.794132102619518</v>
       </c>
       <c r="N10" t="n">
-        <v>2.643204732374711</v>
+        <v>2.643208503723145</v>
       </c>
       <c r="O10" t="n">
-        <v>2.6009371063926</v>
+        <v>2.600940487601541</v>
       </c>
       <c r="P10" t="n">
-        <v>2.654468276283958</v>
+        <v>2.654473174702038</v>
       </c>
       <c r="Q10" t="n">
-        <v>2.816199519417502</v>
+        <v>2.816205631602894</v>
       </c>
       <c r="R10" t="n">
-        <v>3.600202733820135</v>
+        <v>3.600210016424006</v>
       </c>
       <c r="S10" t="n">
-        <v>4.739684278314764</v>
+        <v>4.739694812081077</v>
       </c>
       <c r="T10" t="n">
-        <v>9.372099421241067</v>
+        <v>9.372124086726796</v>
       </c>
       <c r="U10" t="n">
-        <v>2.968636512756348</v>
+        <v>2.968636816198176</v>
       </c>
       <c r="V10" t="n">
-        <v>2.984547701748935</v>
+        <v>2.98454930565574</v>
       </c>
       <c r="W10" t="n">
-        <v>3.065679029984908</v>
+        <v>3.065678986636075</v>
       </c>
       <c r="X10" t="n">
-        <v>3.208517681468617</v>
+        <v>3.208517508073287</v>
       </c>
       <c r="Y10" t="n">
-        <v>3.424823891032826</v>
+        <v>3.424824411218816</v>
       </c>
       <c r="Z10" t="n">
-        <v>4.066863103346392</v>
+        <v>4.066862366416237</v>
       </c>
       <c r="AA10" t="n">
-        <v>5.335608720779419</v>
+        <v>5.335608178919012</v>
       </c>
       <c r="AB10" t="n">
-        <v>9.786421385678379</v>
+        <v>9.786421342329545</v>
       </c>
       <c r="AC10" t="n">
-        <v>4.150200843811035</v>
+        <v>4.150201797485352</v>
       </c>
       <c r="AD10" t="n">
-        <v>5.472358703613281</v>
+        <v>5.472359180450439</v>
       </c>
       <c r="AE10" t="n">
-        <v>6.798209667205811</v>
+        <v>6.798210144042969</v>
       </c>
       <c r="AF10" t="n">
-        <v>8.124359130859375</v>
+        <v>8.124360084533691</v>
       </c>
       <c r="AG10" t="n">
-        <v>9.448772430419922</v>
+        <v>9.448773384094238</v>
       </c>
       <c r="AH10" t="n">
         <v>12.75790786743164</v>
@@ -1711,16 +1907,16 @@
         <v>16.06324577331543</v>
       </c>
       <c r="AJ10" t="n">
-        <v>29.18423461914062</v>
+        <v>29.18423271179199</v>
       </c>
       <c r="AK10" t="n">
-        <v>4.382287502288818</v>
+        <v>4.382288932800293</v>
       </c>
       <c r="AL10" t="n">
-        <v>5.742288112640381</v>
+        <v>5.742289066314697</v>
       </c>
       <c r="AM10" t="n">
-        <v>7.10302734375</v>
+        <v>7.103026866912842</v>
       </c>
       <c r="AN10" t="n">
         <v>8.46346378326416</v>
@@ -1735,7 +1931,31 @@
         <v>16.58949089050293</v>
       </c>
       <c r="AR10" t="n">
-        <v>29.84564971923828</v>
+        <v>29.84565353393555</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>3.100794076919556</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>3.29241943359375</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.341351509094238</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.482970237731934</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>3.847222089767456</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.763570785522461</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.609502792358398</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>9.525020599365234</v>
       </c>
     </row>
     <row r="11">
@@ -1746,118 +1966,118 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.937057106904204</v>
+        <v>3.937056985789079</v>
       </c>
       <c r="D11" t="n">
-        <v>2.470813806037441</v>
+        <v>2.470813613049537</v>
       </c>
       <c r="E11" t="n">
-        <v>3.906845087904547</v>
+        <v>3.906845185817437</v>
       </c>
       <c r="F11" t="n">
-        <v>3.962468862461918</v>
+        <v>3.962468646293287</v>
       </c>
       <c r="G11" t="n">
-        <v>4.100693701276813</v>
+        <v>4.100693661698751</v>
       </c>
       <c r="H11" t="n">
-        <v>4.315285831709261</v>
+        <v>4.315285935511437</v>
       </c>
       <c r="I11" t="n">
-        <v>4.59335647707744</v>
+        <v>4.593356796087346</v>
       </c>
       <c r="J11" t="n">
-        <v>5.499611688643642</v>
+        <v>5.499611451602314</v>
       </c>
       <c r="K11" t="n">
-        <v>6.605150247044222</v>
+        <v>6.605149472528833</v>
       </c>
       <c r="L11" t="n">
-        <v>11.73521295894887</v>
+        <v>11.73521170372587</v>
       </c>
       <c r="M11" t="n">
-        <v>3.731966635123747</v>
+        <v>3.731967074483245</v>
       </c>
       <c r="N11" t="n">
-        <v>3.621919565825852</v>
+        <v>3.621920930331795</v>
       </c>
       <c r="O11" t="n">
-        <v>3.615068333936963</v>
+        <v>3.615069132697866</v>
       </c>
       <c r="P11" t="n">
-        <v>3.714267715155317</v>
+        <v>3.714270107713801</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.909471411814897</v>
+        <v>3.909475426964216</v>
       </c>
       <c r="R11" t="n">
-        <v>4.713191269281344</v>
+        <v>4.713197776547125</v>
       </c>
       <c r="S11" t="n">
-        <v>5.794186397516297</v>
+        <v>5.794197907849608</v>
       </c>
       <c r="T11" t="n">
-        <v>10.66061203538073</v>
+        <v>10.66064004185648</v>
       </c>
       <c r="U11" t="n">
-        <v>3.906845087904547</v>
+        <v>3.906845185817437</v>
       </c>
       <c r="V11" t="n">
-        <v>3.964349703758023</v>
+        <v>3.964350557317037</v>
       </c>
       <c r="W11" t="n">
-        <v>4.103890672792489</v>
+        <v>4.103891448717714</v>
       </c>
       <c r="X11" t="n">
-        <v>4.313685222930101</v>
+        <v>4.313685180199783</v>
       </c>
       <c r="Y11" t="n">
-        <v>4.589756385623913</v>
+        <v>4.589756974599158</v>
       </c>
       <c r="Z11" t="n">
-        <v>5.28704044096205</v>
+        <v>5.287040487083652</v>
       </c>
       <c r="AA11" t="n">
-        <v>6.575636792947262</v>
+        <v>6.575636333993267</v>
       </c>
       <c r="AB11" t="n">
-        <v>11.46671712163497</v>
+        <v>11.46671762574723</v>
       </c>
       <c r="AC11" t="n">
-        <v>4.96037075379822</v>
+        <v>4.960371330574216</v>
       </c>
       <c r="AD11" t="n">
-        <v>6.102749014356282</v>
+        <v>6.10274963943476</v>
       </c>
       <c r="AE11" t="n">
-        <v>7.309107066671041</v>
+        <v>7.309107327626118</v>
       </c>
       <c r="AF11" t="n">
-        <v>8.552379558108786</v>
+        <v>8.552380450187309</v>
       </c>
       <c r="AG11" t="n">
-        <v>9.817182650603609</v>
+        <v>9.817183039177126</v>
       </c>
       <c r="AH11" t="n">
-        <v>13.0344351482444</v>
+        <v>13.03443690422245</v>
       </c>
       <c r="AI11" t="n">
-        <v>16.2917057957224</v>
+        <v>16.29170673232099</v>
       </c>
       <c r="AJ11" t="n">
         <v>29.37514232844509</v>
       </c>
       <c r="AK11" t="n">
-        <v>5.048823402741989</v>
+        <v>5.048824536084314</v>
       </c>
       <c r="AL11" t="n">
-        <v>6.26088621015225</v>
+        <v>6.260887733377826</v>
       </c>
       <c r="AM11" t="n">
         <v>7.52526516367971</v>
       </c>
       <c r="AN11" t="n">
-        <v>8.819041320184915</v>
+        <v>8.819042185289623</v>
       </c>
       <c r="AO11" t="n">
         <v>10.12931524555091</v>
@@ -1870,6 +2090,30 @@
       </c>
       <c r="AR11" t="n">
         <v>30.04709539863265</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>4.011226397260943</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4.212107536529901</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>4.260438777552203</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4.49664626716151</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>4.865197523445341</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>6.120555900309105</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>7.215306373060599</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>12.11422281994392</v>
       </c>
     </row>
     <row r="12">
@@ -1886,67 +2130,67 @@
         <v>0.999891459941864</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9997859597206116</v>
+        <v>0.9997857213020325</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9997707009315491</v>
+        <v>0.9997705817222595</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9997439384460449</v>
+        <v>0.9997438192367554</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9997050762176514</v>
+        <v>0.9997049570083618</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9996550679206848</v>
+        <v>0.9996548295021057</v>
       </c>
       <c r="J12" t="n">
         <v>0.9994794130325317</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9992312788963318</v>
+        <v>0.9992311596870422</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9975290298461914</v>
+        <v>0.9975289702415466</v>
       </c>
       <c r="M12" t="n">
         <v>0.999788761138916</v>
       </c>
       <c r="N12" t="n">
-        <v>0.9997825622558594</v>
+        <v>0.999782383441925</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9997703433036804</v>
+        <v>0.9997702836990356</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9997521638870239</v>
+        <v>0.9997519850730896</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.9997276663780212</v>
+        <v>0.9997274279594421</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9996398687362671</v>
+        <v>0.999639630317688</v>
       </c>
       <c r="S12" t="n">
-        <v>0.999508798122406</v>
+        <v>0.9995086789131165</v>
       </c>
       <c r="T12" t="n">
-        <v>0.9985557198524475</v>
+        <v>0.9985556602478027</v>
       </c>
       <c r="U12" t="n">
-        <v>0.9997859597206116</v>
+        <v>0.9997857213020325</v>
       </c>
       <c r="V12" t="n">
-        <v>0.9997708201408386</v>
+        <v>0.9997707009315491</v>
       </c>
       <c r="W12" t="n">
-        <v>0.9997444152832031</v>
+        <v>0.9997442960739136</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9997075796127319</v>
+        <v>0.9997074604034424</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.9996593594551086</v>
+        <v>0.9996592402458191</v>
       </c>
       <c r="Z12" t="n">
         <v>0.999530017375946</v>
@@ -1955,59 +2199,83 @@
         <v>0.9992551803588867</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.9977893829345703</v>
+        <v>0.9977893233299255</v>
       </c>
       <c r="AC12" t="n">
         <v>0.9997064471244812</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.9995900392532349</v>
+        <v>0.9995899796485901</v>
       </c>
       <c r="AE12" t="n">
         <v>0.9994386434555054</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.9992522001266479</v>
+        <v>0.9992522597312927</v>
       </c>
       <c r="AG12" t="n">
         <v>0.9990307092666626</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.9983126521110535</v>
+        <v>0.998312771320343</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.9973470568656921</v>
+        <v>0.9973469376564026</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.9907602071762085</v>
+        <v>0.9907600879669189</v>
       </c>
       <c r="AK12" t="n">
         <v>0.9996626973152161</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.9994825124740601</v>
+        <v>0.999482274055481</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.9992474317550659</v>
+        <v>0.9992472529411316</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.9989569187164307</v>
+        <v>0.9989567399024963</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.9986106753349304</v>
+        <v>0.9986105561256409</v>
       </c>
       <c r="AP12" t="n">
-        <v>0.9974929690361023</v>
+        <v>0.9974929094314575</v>
       </c>
       <c r="AQ12" t="n">
-        <v>0.9960033893585205</v>
+        <v>0.996003270149231</v>
       </c>
       <c r="AR12" t="n">
         <v>0.9862581491470337</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997820258140564</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.9997525215148926</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997411370277405</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996987581253052</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9996479153633118</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9994039535522461</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9991762042045593</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9975077509880066</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>